<commit_message>
implemented fill form method
</commit_message>
<xml_diff>
--- a/core/src/test/resources/TestData_FF.xlsx
+++ b/core/src/test/resources/TestData_FF.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4514\IdeaProjects\java-endtoend-fw\core\src\main\java\core\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4514\IdeaProjects\java-endtoend-fw\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CB5E88-26FE-43F6-B961-2F8DE6F851DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2C8B55-47F3-471C-A98F-F819757AAF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>Lname2</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
+    <t>#fname</t>
+  </si>
+  <si>
+    <t>#lname</t>
   </si>
 </sst>
 </file>
@@ -416,18 +425,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06BCC99-81A5-49E9-B1A4-893852FF5E73}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,13 +445,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -449,13 +462,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -463,9 +479,12 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a sample test case with dataflow
</commit_message>
<xml_diff>
--- a/core/src/test/resources/TestData_FF.xlsx
+++ b/core/src/test/resources/TestData_FF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4514\IdeaProjects\java-endtoend-fw\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2C8B55-47F3-471C-A98F-F819757AAF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4EBB0B-9466-4791-8282-93D718A0CE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -70,20 +70,37 @@
     <t>Locator</t>
   </si>
   <si>
-    <t>#fname</t>
-  </si>
-  <si>
-    <t>#lname</t>
+    <t>#firstName</t>
+  </si>
+  <si>
+    <t>#lastName</t>
+  </si>
+  <si>
+    <t>#userEmail</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>autom@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,13 +123,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,16 +445,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06BCC99-81A5-49E9-B1A4-893852FF5E73}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.3671875" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -488,8 +509,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{764492C0-6702-44C6-9307-F08F90D46A64}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added code to build test from cmd
</commit_message>
<xml_diff>
--- a/core/src/test/resources/TestData_FF.xlsx
+++ b/core/src/test/resources/TestData_FF.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4514\IdeaProjects\java-endtoend-fw\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4EBB0B-9466-4791-8282-93D718A0CE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CABFB40-0D70-4B6A-8135-6233AF3BBC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -445,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06BCC99-81A5-49E9-B1A4-893852FF5E73}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -509,28 +510,54 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F393EF-3107-4569-8DDB-DB44D3687E05}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{764492C0-6702-44C6-9307-F08F90D46A64}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{764492C0-6702-44C6-9307-F08F90D46A64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed locator type casing
</commit_message>
<xml_diff>
--- a/core/src/test/resources/TestData_FF.xlsx
+++ b/core/src/test/resources/TestData_FF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4514\IdeaProjects\java-endtoend-fw\core\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CABFB40-0D70-4B6A-8135-6233AF3BBC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4469CB94-F701-4583-8D67-987BA9B58CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{2177194E-30AC-483F-8DB9-AE02475C28FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Question</t>
   </si>
@@ -50,9 +50,6 @@
     <t>TC02</t>
   </si>
   <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Textbox</t>
   </si>
   <si>
@@ -71,19 +68,103 @@
     <t>Locator</t>
   </si>
   <si>
-    <t>#firstName</t>
-  </si>
-  <si>
-    <t>#lastName</t>
-  </si>
-  <si>
-    <t>#userEmail</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>autom@gmail.com</t>
+    <t>LocatorType</t>
+  </si>
+  <si>
+    <t>CssSelector</t>
+  </si>
+  <si>
+    <t>cssSelector</t>
+  </si>
+  <si>
+    <t>#email</t>
+  </si>
+  <si>
+    <t>#fname</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>14 Silverwattle Drive , Melbourne</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>#city</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>#state</t>
+  </si>
+  <si>
+    <t>#zip</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>Name On Card</t>
+  </si>
+  <si>
+    <t>Auto User</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>#expmonth</t>
+  </si>
+  <si>
+    <t>#expyear</t>
+  </si>
+  <si>
+    <t>Expiry Month</t>
+  </si>
+  <si>
+    <t>Expiry Year</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>//input[@id='cvv']</t>
+  </si>
+  <si>
+    <t>Januaray</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>42556566522266500</t>
+  </si>
+  <si>
+    <t>3008</t>
+  </si>
+  <si>
+    <t>#adr</t>
+  </si>
+  <si>
+    <t>#cname</t>
+  </si>
+  <si>
+    <t>#ccnum</t>
   </si>
 </sst>
 </file>
@@ -115,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,14 +204,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,20 +538,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06BCC99-81A5-49E9-B1A4-893852FF5E73}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3671875" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.3671875" customWidth="1"/>
+    <col min="5" max="5" width="27.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,47 +559,109 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -518,46 +672,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F393EF-3107-4569-8DDB-DB44D3687E05}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7890625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{764492C0-6702-44C6-9307-F08F90D46A64}"/>
+    <hyperlink ref="E2" r:id="rId1" display="autom@gmail.com" xr:uid="{764492C0-6702-44C6-9307-F08F90D46A64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>